<commit_message>
upgraded to version 1.10.0.1
</commit_message>
<xml_diff>
--- a/data/xlsx/cis.xlsx
+++ b/data/xlsx/cis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jww/Developer/python/terraformer/data/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB18C492-6A1C-EF41-9DF0-7012D47B9D7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DC8FD34-D09D-3142-8D2D-F8CBF514972B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14780" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14780" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cisinstances" sheetId="50" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="74">
   <si>
     <t>*name</t>
   </si>
@@ -85,15 +85,6 @@
     <t>var.domain</t>
   </si>
   <si>
-    <t># Retrieve CIS instance data</t>
-  </si>
-  <si>
-    <t># Define CIS domains</t>
-  </si>
-  <si>
-    <t># Define CIS health checks for nginx</t>
-  </si>
-  <si>
     <t>root</t>
   </si>
   <si>
@@ -142,9 +133,6 @@
     <t>"Websiteroot"</t>
   </si>
   <si>
-    <t># Create pool (of one) with VPC LBaaS instances using URL</t>
-  </si>
-  <si>
     <t>*origins.name</t>
   </si>
   <si>
@@ -187,9 +175,6 @@
     <t>"true"</t>
   </si>
   <si>
-    <t># Define GLB name advertised by DNS for the website: prefix + domain, and enable DDOS</t>
-  </si>
-  <si>
     <t>*domain_id</t>
   </si>
   <si>
@@ -254,6 +239,24 @@
   </si>
   <si>
     <t>session_affinity</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>Retrieve CIS instance data</t>
+  </si>
+  <si>
+    <t>Define CIS domains</t>
+  </si>
+  <si>
+    <t>Define CIS health checks for nginx</t>
+  </si>
+  <si>
+    <t>Create pool (of one) with VPC LBaaS instances using URL</t>
+  </si>
+  <si>
+    <t>Define GLB name advertised by DNS for the website: prefix + domain, and enable DDOS</t>
   </si>
 </sst>
 </file>
@@ -344,7 +347,10 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="48">
+  <dxfs count="52">
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -435,6 +441,9 @@
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -517,12 +526,18 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="4"/>
         </patternFill>
       </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -591,100 +606,105 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{2ECE5DB1-D260-6E49-B492-4FB9F047A792}" name="Table3" displayName="Table3" ref="A1:G6" totalsRowShown="0" headerRowDxfId="47">
-  <autoFilter ref="A1:G6" xr:uid="{BF7B2943-D8B2-F141-A648-1F77292E609F}"/>
-  <tableColumns count="7">
-    <tableColumn id="9" xr3:uid="{EF22B46C-EEC8-954B-9006-F5C934140BA4}" name="*file" dataDxfId="46"/>
-    <tableColumn id="8" xr3:uid="{14BCF91D-C69D-4A48-BAE6-6FE0CE708F39}" name="*resource" dataDxfId="45"/>
-    <tableColumn id="1" xr3:uid="{7E74D83A-54A4-D149-81D3-7E89BF180D8D}" name="*name" dataDxfId="44"/>
-    <tableColumn id="2" xr3:uid="{C8993A1E-13ED-9646-B484-5C8D98EE5999}" name="*plan" dataDxfId="43"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{2ECE5DB1-D260-6E49-B492-4FB9F047A792}" name="Table3" displayName="Table3" ref="A1:H4" totalsRowShown="0" headerRowDxfId="51">
+  <autoFilter ref="A1:H4" xr:uid="{BF7B2943-D8B2-F141-A648-1F77292E609F}"/>
+  <tableColumns count="8">
+    <tableColumn id="9" xr3:uid="{EF22B46C-EEC8-954B-9006-F5C934140BA4}" name="*file" dataDxfId="50"/>
+    <tableColumn id="8" xr3:uid="{14BCF91D-C69D-4A48-BAE6-6FE0CE708F39}" name="*resource" dataDxfId="49"/>
+    <tableColumn id="1" xr3:uid="{7E74D83A-54A4-D149-81D3-7E89BF180D8D}" name="*name" dataDxfId="48"/>
+    <tableColumn id="2" xr3:uid="{C8993A1E-13ED-9646-B484-5C8D98EE5999}" name="*plan" dataDxfId="47"/>
     <tableColumn id="3" xr3:uid="{E05E3D1A-B4E0-144E-B4A0-2A74FB710BE1}" name="*location"/>
     <tableColumn id="4" xr3:uid="{F53EAA06-1D92-0941-BD62-CFA25A63B0D9}" name="resource_group_id"/>
     <tableColumn id="7" xr3:uid="{2524A41E-F007-AE48-9710-277646E4A10F}" name="tags"/>
+    <tableColumn id="5" xr3:uid="{4FA1D7D3-8773-4B4B-A13F-A360E6B98F88}" name="comments"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{94CB4938-803E-6A45-818C-239D4C2D3032}" name="Table14" displayName="Table14" ref="A1:D6" totalsRowShown="0" headerRowDxfId="42">
-  <autoFilter ref="A1:D6" xr:uid="{E37DA650-CD8A-9248-A324-C4E06B2EFAF3}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{94CB4938-803E-6A45-818C-239D4C2D3032}" name="Table14" displayName="Table14" ref="A1:E4" totalsRowShown="0" headerRowDxfId="46">
+  <autoFilter ref="A1:E4" xr:uid="{E37DA650-CD8A-9248-A324-C4E06B2EFAF3}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{B213F9EA-EE5C-F141-83B8-5F805CCFF0B8}" name="*file"/>
     <tableColumn id="11" xr3:uid="{BD2203B1-67E0-C748-8240-2DAB0412E863}" name="*resource"/>
-    <tableColumn id="2" xr3:uid="{58502468-21D1-1040-A10E-00FB04A9B10A}" name="*domain" dataDxfId="41"/>
-    <tableColumn id="3" xr3:uid="{36A4DC5F-3D00-1742-BF10-5AE11EE1736D}" name="*cis_id" dataDxfId="40"/>
+    <tableColumn id="2" xr3:uid="{58502468-21D1-1040-A10E-00FB04A9B10A}" name="*domain" dataDxfId="45"/>
+    <tableColumn id="3" xr3:uid="{36A4DC5F-3D00-1742-BF10-5AE11EE1736D}" name="*cis_id" dataDxfId="44"/>
+    <tableColumn id="4" xr3:uid="{28BF7EF6-2A3C-9947-93F1-F617473E1721}" name="comments" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{85162D83-2223-2743-94A8-CBB5DCABF5E2}" name="Table5" displayName="Table5" ref="A1:O6" totalsRowShown="0" headerRowDxfId="39">
-  <autoFilter ref="A1:O6" xr:uid="{BABC147B-328A-9E42-A692-B07DDF9AA10A}"/>
-  <tableColumns count="15">
-    <tableColumn id="16" xr3:uid="{878D88ED-76D1-9E45-AFBB-45E26283A42D}" name="*file" dataDxfId="38"/>
-    <tableColumn id="17" xr3:uid="{76B528BC-6979-CD40-AA48-F7EF2765CC75}" name="*resource" dataDxfId="37"/>
-    <tableColumn id="1" xr3:uid="{1A08DB6B-DC44-4B4A-ACBB-35F1471E6D94}" name="*cis_id" dataDxfId="36"/>
-    <tableColumn id="2" xr3:uid="{20D213A0-12B0-A448-93A2-6A4F802B619E}" name="*expected_body" dataDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{C8D92085-C2A2-E94B-9427-75ADBDD22F85}" name="*expected_codes" dataDxfId="34"/>
-    <tableColumn id="4" xr3:uid="{B3053301-5B4F-4F45-9DF1-DA16E8095157}" name="allow_insecure" dataDxfId="33"/>
-    <tableColumn id="5" xr3:uid="{7C332576-C537-4248-9FF0-2F9304672F27}" name="follow_redirects" dataDxfId="32"/>
-    <tableColumn id="6" xr3:uid="{510D5DA4-96D6-9949-8E0A-ACCD7802CF77}" name="method" dataDxfId="31"/>
-    <tableColumn id="7" xr3:uid="{FADE0027-F404-2A4B-B748-0B5DED401559}" name="timeout" dataDxfId="30"/>
-    <tableColumn id="8" xr3:uid="{48E221A6-8A70-8F49-9024-3BB8C6AB4DA4}" name="path" dataDxfId="29"/>
-    <tableColumn id="9" xr3:uid="{DFCC5FFE-E582-F04E-A8A9-916B566859A5}" name="port" dataDxfId="28" dataCellStyle="Hyperlink"/>
-    <tableColumn id="15" xr3:uid="{FDF5BBAA-A030-0249-B742-785E3947CFDE}" name="interval" dataDxfId="27" dataCellStyle="Hyperlink"/>
-    <tableColumn id="10" xr3:uid="{4A2772BB-820B-5A45-8BFB-F7F0C1B6AB42}" name="retries" dataDxfId="26"/>
-    <tableColumn id="13" xr3:uid="{A27FBA85-3106-504B-9F02-448FD69509DA}" name="type" dataDxfId="25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{85162D83-2223-2743-94A8-CBB5DCABF5E2}" name="Table5" displayName="Table5" ref="A1:P4" totalsRowShown="0" headerRowDxfId="42">
+  <autoFilter ref="A1:P4" xr:uid="{BABC147B-328A-9E42-A692-B07DDF9AA10A}"/>
+  <tableColumns count="16">
+    <tableColumn id="16" xr3:uid="{878D88ED-76D1-9E45-AFBB-45E26283A42D}" name="*file" dataDxfId="41"/>
+    <tableColumn id="17" xr3:uid="{76B528BC-6979-CD40-AA48-F7EF2765CC75}" name="*resource" dataDxfId="40"/>
+    <tableColumn id="1" xr3:uid="{1A08DB6B-DC44-4B4A-ACBB-35F1471E6D94}" name="*cis_id" dataDxfId="39"/>
+    <tableColumn id="2" xr3:uid="{20D213A0-12B0-A448-93A2-6A4F802B619E}" name="*expected_body" dataDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{C8D92085-C2A2-E94B-9427-75ADBDD22F85}" name="*expected_codes" dataDxfId="37"/>
+    <tableColumn id="4" xr3:uid="{B3053301-5B4F-4F45-9DF1-DA16E8095157}" name="allow_insecure" dataDxfId="36"/>
+    <tableColumn id="5" xr3:uid="{7C332576-C537-4248-9FF0-2F9304672F27}" name="follow_redirects" dataDxfId="35"/>
+    <tableColumn id="6" xr3:uid="{510D5DA4-96D6-9949-8E0A-ACCD7802CF77}" name="method" dataDxfId="34"/>
+    <tableColumn id="7" xr3:uid="{FADE0027-F404-2A4B-B748-0B5DED401559}" name="timeout" dataDxfId="33"/>
+    <tableColumn id="8" xr3:uid="{48E221A6-8A70-8F49-9024-3BB8C6AB4DA4}" name="path" dataDxfId="32"/>
+    <tableColumn id="9" xr3:uid="{DFCC5FFE-E582-F04E-A8A9-916B566859A5}" name="port" dataDxfId="31" dataCellStyle="Hyperlink"/>
+    <tableColumn id="15" xr3:uid="{FDF5BBAA-A030-0249-B742-785E3947CFDE}" name="interval" dataDxfId="30" dataCellStyle="Hyperlink"/>
+    <tableColumn id="10" xr3:uid="{4A2772BB-820B-5A45-8BFB-F7F0C1B6AB42}" name="retries" dataDxfId="29"/>
+    <tableColumn id="13" xr3:uid="{A27FBA85-3106-504B-9F02-448FD69509DA}" name="type" dataDxfId="28"/>
     <tableColumn id="14" xr3:uid="{6B54822D-58A6-6944-8211-A034328AAF7F}" name="description"/>
+    <tableColumn id="11" xr3:uid="{543A669D-4596-444D-A245-4E9CFD6846C1}" name="comments" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{398DB5A6-1B4D-6846-8DA7-E5AD59B6CE38}" name="Table13" displayName="Table13" ref="A1:M7" totalsRowShown="0" headerRowDxfId="24">
-  <autoFilter ref="A1:M7" xr:uid="{84D85FF3-D4A2-A145-9664-43C3D0B8D1F9}"/>
-  <tableColumns count="13">
-    <tableColumn id="11" xr3:uid="{28A3F32E-57F6-8842-B2B2-A04B774CDA50}" name="*file" dataDxfId="23"/>
-    <tableColumn id="1" xr3:uid="{057B1271-2391-7841-A672-9AD2C1910205}" name="*resource" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{F2654A05-284B-0140-951D-DB928685A88A}" name="*name" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{6B716C5D-FF66-C746-8CFC-062268AAF158}" name="*cis_id" dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{DD77321C-9398-EE40-BFFA-ECD6F45DA631}" name="*origins.name" dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{6D9BEBF8-3CC8-4A46-B1C0-8CAEB4F85B2B}" name="*origins.address" dataDxfId="18"/>
-    <tableColumn id="7" xr3:uid="{F8E3EE05-E616-E84F-99DB-97543EF6C5C8}" name="origins.enabled" dataDxfId="17"/>
-    <tableColumn id="8" xr3:uid="{2CB92F37-5516-0349-A041-0758DAC69BB1}" name="check_regions" dataDxfId="16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{398DB5A6-1B4D-6846-8DA7-E5AD59B6CE38}" name="Table13" displayName="Table13" ref="A1:N5" totalsRowShown="0" headerRowDxfId="26">
+  <autoFilter ref="A1:N5" xr:uid="{84D85FF3-D4A2-A145-9664-43C3D0B8D1F9}"/>
+  <tableColumns count="14">
+    <tableColumn id="11" xr3:uid="{28A3F32E-57F6-8842-B2B2-A04B774CDA50}" name="*file" dataDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{057B1271-2391-7841-A672-9AD2C1910205}" name="*resource" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{F2654A05-284B-0140-951D-DB928685A88A}" name="*name" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{6B716C5D-FF66-C746-8CFC-062268AAF158}" name="*cis_id" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{DD77321C-9398-EE40-BFFA-ECD6F45DA631}" name="*origins.name" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{6D9BEBF8-3CC8-4A46-B1C0-8CAEB4F85B2B}" name="*origins.address" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{F8E3EE05-E616-E84F-99DB-97543EF6C5C8}" name="origins.enabled" dataDxfId="19"/>
+    <tableColumn id="8" xr3:uid="{2CB92F37-5516-0349-A041-0758DAC69BB1}" name="check_regions" dataDxfId="18"/>
     <tableColumn id="9" xr3:uid="{C52E3E2D-54DD-9446-B067-67A8B4C63FC4}" name="*enabled"/>
-    <tableColumn id="12" xr3:uid="{3BCB8C14-313C-5C47-B338-1C3B34555847}" name="minimum_origins" dataDxfId="15"/>
-    <tableColumn id="14" xr3:uid="{61132B2B-CE67-0142-8238-8B40F442C239}" name="monitor" dataDxfId="14"/>
-    <tableColumn id="15" xr3:uid="{12406BFC-CA2F-7646-9250-D1E6593C5496}" name="notification_email" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{CA6B29A9-8DBA-A141-9A3E-DB021D547D4B}" name="description" dataDxfId="12"/>
+    <tableColumn id="12" xr3:uid="{3BCB8C14-313C-5C47-B338-1C3B34555847}" name="minimum_origins" dataDxfId="17"/>
+    <tableColumn id="14" xr3:uid="{61132B2B-CE67-0142-8238-8B40F442C239}" name="monitor" dataDxfId="16"/>
+    <tableColumn id="15" xr3:uid="{12406BFC-CA2F-7646-9250-D1E6593C5496}" name="notification_email" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{CA6B29A9-8DBA-A141-9A3E-DB021D547D4B}" name="description" dataDxfId="14"/>
+    <tableColumn id="10" xr3:uid="{D6209E72-2397-5E4A-A0D8-2DE5E021EFC5}" name="comments" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E60FD6E6-8DD8-8245-8578-34024AB794A8}" name="Table142" displayName="Table142" ref="A1:P6" totalsRowShown="0" headerRowDxfId="11">
-  <autoFilter ref="A1:P6" xr:uid="{E37DA650-CD8A-9248-A324-C4E06B2EFAF3}"/>
-  <tableColumns count="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E60FD6E6-8DD8-8245-8578-34024AB794A8}" name="Table142" displayName="Table142" ref="A1:Q4" totalsRowShown="0" headerRowDxfId="12">
+  <autoFilter ref="A1:Q4" xr:uid="{E37DA650-CD8A-9248-A324-C4E06B2EFAF3}"/>
+  <tableColumns count="17">
     <tableColumn id="9" xr3:uid="{E289064D-9E30-6C4C-8CE3-2300AC9C55C4}" name="*file"/>
     <tableColumn id="8" xr3:uid="{8F49C81B-5D52-C346-A10B-A5E168959794}" name="*resource"/>
     <tableColumn id="1" xr3:uid="{2FF8BFB2-91EE-A446-86F9-74CD2B7E4EAB}" name="*name"/>
-    <tableColumn id="2" xr3:uid="{2D2B65B1-D705-9545-9296-FDE0CA8FE849}" name="*domain_id" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{953F377D-3690-9F49-A2D7-13E4CAED4CFD}" name="*cis_id" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{98E5F21F-122F-974A-BFBE-71CD3158F486}" name="*fallback_pool_id" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{59A20E18-E999-CA42-A9C6-78B5F8A5066C}" name="*default_pool_ids" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{2D2B65B1-D705-9545-9296-FDE0CA8FE849}" name="*domain_id" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{953F377D-3690-9F49-A2D7-13E4CAED4CFD}" name="*cis_id" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{98E5F21F-122F-974A-BFBE-71CD3158F486}" name="*fallback_pool_id" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{59A20E18-E999-CA42-A9C6-78B5F8A5066C}" name="*default_pool_ids" dataDxfId="8"/>
     <tableColumn id="7" xr3:uid="{91140738-BFFB-CB49-8086-4F979E2D8C20}" name="enabled"/>
     <tableColumn id="10" xr3:uid="{EE53A3E3-AC51-2E45-94FD-5B629F7F4A61}" name="proxied"/>
-    <tableColumn id="11" xr3:uid="{A4418ECD-257B-A84B-9215-A5037C57B73E}" name="ttl" dataDxfId="6"/>
-    <tableColumn id="12" xr3:uid="{3960BBEB-542E-134A-A0F1-81379627FFD9}" name="region_pools.region" dataDxfId="5"/>
-    <tableColumn id="13" xr3:uid="{FB0B11AB-1D3B-8647-B2AF-6D78B6FE0980}" name="region_pools.pool_ids" dataDxfId="4"/>
-    <tableColumn id="14" xr3:uid="{37DAD431-C8FE-8144-8EC6-DB2614B75275}" name="pop_pools.pop" dataDxfId="3"/>
-    <tableColumn id="15" xr3:uid="{1797F1A8-7BF5-734E-B521-4B8C202F3DE2}" name="pop_pools.pool_ids" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{34FED888-0789-3744-99EB-22BDC378ABB8}" name="session_affinity" dataDxfId="1"/>
-    <tableColumn id="16" xr3:uid="{2C208C8E-EE86-0245-93AE-B5B5D563BA3D}" name="description" dataDxfId="0"/>
+    <tableColumn id="11" xr3:uid="{A4418ECD-257B-A84B-9215-A5037C57B73E}" name="ttl" dataDxfId="7"/>
+    <tableColumn id="12" xr3:uid="{3960BBEB-542E-134A-A0F1-81379627FFD9}" name="region_pools.region" dataDxfId="6"/>
+    <tableColumn id="13" xr3:uid="{FB0B11AB-1D3B-8647-B2AF-6D78B6FE0980}" name="region_pools.pool_ids" dataDxfId="5"/>
+    <tableColumn id="14" xr3:uid="{37DAD431-C8FE-8144-8EC6-DB2614B75275}" name="pop_pools.pop" dataDxfId="4"/>
+    <tableColumn id="15" xr3:uid="{1797F1A8-7BF5-734E-B521-4B8C202F3DE2}" name="pop_pools.pool_ids" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{34FED888-0789-3744-99EB-22BDC378ABB8}" name="session_affinity" dataDxfId="2"/>
+    <tableColumn id="16" xr3:uid="{2C208C8E-EE86-0245-93AE-B5B5D563BA3D}" name="description" dataDxfId="1"/>
+    <tableColumn id="17" xr3:uid="{82708A7F-4AE6-D348-B3A4-04A98F900B67}" name="comments" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -953,24 +973,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3B909B7-5B7F-FE4A-8CD8-0D8F5B038E31}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" customWidth="1"/>
+    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
@@ -992,52 +1011,44 @@
       <c r="G1" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="H1" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1049,17 +1060,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{711B9366-0593-C248-9411-B78B3C2D6CE0}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" customWidth="1"/>
+    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
@@ -1068,7 +1079,7 @@
     <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -1081,39 +1092,36 @@
       <c r="D1" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
+      <c r="E1" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1125,13 +1133,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA16B708-803A-4C41-87F9-C6AEEBD9524B}">
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" customWidth="1"/>
+    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
@@ -1146,11 +1156,11 @@
     <col min="13" max="13" width="8.83203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
@@ -1161,63 +1171,81 @@
         <v>14</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
+      <c r="J2" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="O2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -1232,71 +1260,25 @@
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="P3" s="1"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-      <c r="J4" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="J4" s="1"/>
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
-      <c r="O4" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1308,15 +1290,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F060F451-DD45-A340-881E-50BF9BBCCEF3}">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" customWidth="1"/>
+    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.1640625" bestFit="1" customWidth="1"/>
@@ -1329,10 +1309,10 @@
     <col min="11" max="11" width="23.1640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="43.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -1346,52 +1326,76 @@
         <v>14</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="M1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="D2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
+      <c r="K2" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
-        <v>35</v>
-      </c>
+      <c r="N2" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -1404,85 +1408,38 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>49</v>
-      </c>
+      <c r="N3" s="1"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-      <c r="K4" s="1" t="s">
-        <v>70</v>
-      </c>
+      <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
+      <c r="N4" s="1"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
+      <c r="N5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1494,13 +1451,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{014ADAAB-5E2C-2345-B6AB-833E609C1DAB}">
-  <dimension ref="A1:P6"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" customWidth="1"/>
+    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32" bestFit="1" customWidth="1"/>
@@ -1516,9 +1473,10 @@
     <col min="14" max="14" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="67" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -1529,63 +1487,89 @@
         <v>0</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="H1" s="4" t="s">
+      <c r="M1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="O1" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
         <v>55</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="C2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="G2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="M1" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="I2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>50</v>
-      </c>
+      <c r="O2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -1598,71 +1582,22 @@
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>49</v>
-      </c>
+      <c r="Q3" s="1"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
-      <c r="O4" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>